<commit_message>
bug fix re create shift and change template
</commit_message>
<xml_diff>
--- a/public/static/templates/Onshift_Employee_Template.xlsx
+++ b/public/static/templates/Onshift_Employee_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arifw\Dropbox\PC\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C71F2A-1BF1-4751-81C5-864A637B0F5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4622E776-BB56-4798-9DC8-C504F75B71C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6315" yWindow="2370" windowWidth="28800" windowHeight="15345" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>EMPLOYEE LIST</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>Phone Number</t>
-  </si>
-  <si>
-    <t>Platform</t>
   </si>
 </sst>
 </file>
@@ -527,7 +524,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -563,9 +560,6 @@
       <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="4" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
@@ -575,7 +569,6 @@
       <c r="C4" s="4"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
@@ -585,7 +578,6 @@
       <c r="C5" s="4"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
@@ -595,7 +587,6 @@
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
@@ -605,7 +596,6 @@
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
@@ -615,7 +605,6 @@
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
@@ -625,7 +614,6 @@
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
@@ -635,7 +623,6 @@
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
@@ -645,7 +632,6 @@
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
@@ -655,7 +641,6 @@
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
@@ -665,7 +650,6 @@
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
@@ -675,7 +659,6 @@
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
@@ -685,7 +668,6 @@
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
@@ -695,9 +677,8 @@
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>14</v>
       </c>
@@ -705,9 +686,8 @@
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>15</v>
       </c>
@@ -715,9 +695,8 @@
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>16</v>
       </c>
@@ -725,9 +704,8 @@
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>17</v>
       </c>
@@ -735,9 +713,8 @@
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>18</v>
       </c>
@@ -745,9 +722,8 @@
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-    </row>
-    <row r="22" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>19</v>
       </c>
@@ -755,9 +731,8 @@
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-    </row>
-    <row r="23" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>20</v>
       </c>
@@ -765,9 +740,8 @@
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-    </row>
-    <row r="24" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>21</v>
       </c>
@@ -775,9 +749,8 @@
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-    </row>
-    <row r="25" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>22</v>
       </c>
@@ -785,9 +758,8 @@
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-    </row>
-    <row r="26" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>23</v>
       </c>
@@ -795,9 +767,8 @@
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-    </row>
-    <row r="27" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>24</v>
       </c>
@@ -805,9 +776,8 @@
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-    </row>
-    <row r="28" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>25</v>
       </c>
@@ -815,9 +785,8 @@
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-    </row>
-    <row r="29" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    </row>
+    <row r="29" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="D1:F1"/>

</xml_diff>